<commit_message>
Added another LRM change in NS 1 (From Y to N)
</commit_message>
<xml_diff>
--- a/Data v2.xlsx
+++ b/Data v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katli\RWA Explain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katli\RWA Explain\RWA_Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{28FE514F-BA6B-4993-B2B6-5D4053CB4307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D998E63-6462-4373-902B-EDC794280648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9915" yWindow="0" windowWidth="18990" windowHeight="15585" activeTab="1" xr2:uid="{43B1DDD3-62A0-4D36-B06F-A84F66130CB3}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{43B1DDD3-62A0-4D36-B06F-A84F66130CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,25 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_1!$A$1:$BT$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data_2!$A$1:$BT$45</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1041,10 +1054,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1423,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE6C133-E1A4-4714-9385-C25DA1CAD29C}">
   <dimension ref="A1:BT45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1445,7 @@
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="52" max="66" width="9.140625" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="9.140625" customWidth="1"/>
-    <col min="68" max="68" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.25">
@@ -1637,7 +1650,7 @@
       <c r="BO1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BP1" s="3" t="s">
         <v>67</v>
       </c>
       <c r="BQ1" t="s">
@@ -1854,7 +1867,7 @@
       <c r="BN2">
         <v>18000</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="4">
         <v>891186.97</v>
       </c>
       <c r="BQ2">
@@ -2071,7 +2084,7 @@
       <c r="BN3">
         <v>8000</v>
       </c>
-      <c r="BP3">
+      <c r="BP3" s="4">
         <v>113431.08</v>
       </c>
       <c r="BQ3">
@@ -2291,7 +2304,7 @@
       <c r="BN4">
         <v>1000</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="4">
         <v>14744.43</v>
       </c>
       <c r="BQ4">
@@ -2508,7 +2521,7 @@
       <c r="BN5">
         <v>7000</v>
       </c>
-      <c r="BP5">
+      <c r="BP5" s="4">
         <v>324680.8</v>
       </c>
       <c r="BQ5">
@@ -2725,7 +2738,7 @@
       <c r="BN6">
         <v>20000</v>
       </c>
-      <c r="BP6">
+      <c r="BP6" s="4">
         <v>4850034.55</v>
       </c>
       <c r="BQ6">
@@ -2934,9 +2947,9 @@
         <v>88</v>
       </c>
       <c r="BO7">
-        <v>980316320.20000005</v>
-      </c>
-      <c r="BP7"/>
+        <v>18031632.199999999</v>
+      </c>
+      <c r="BP7" s="4"/>
       <c r="BQ7">
         <v>0</v>
       </c>
@@ -3148,7 +3161,7 @@
       <c r="BN8">
         <v>50000</v>
       </c>
-      <c r="BP8" s="2">
+      <c r="BP8" s="4">
         <v>12396987.9</v>
       </c>
       <c r="BQ8">
@@ -3362,7 +3375,7 @@
       <c r="BN9">
         <v>119912</v>
       </c>
-      <c r="BP9" s="2">
+      <c r="BP9" s="4">
         <v>11103288</v>
       </c>
       <c r="BQ9">
@@ -3579,7 +3592,7 @@
       <c r="BN10">
         <v>129819</v>
       </c>
-      <c r="BP10" s="2">
+      <c r="BP10" s="4">
         <v>15094847.359999999</v>
       </c>
       <c r="BQ10">
@@ -3793,7 +3806,7 @@
       <c r="BN11">
         <v>21124</v>
       </c>
-      <c r="BP11" s="2">
+      <c r="BP11" s="4">
         <v>5849007.2999999998</v>
       </c>
       <c r="BQ11">
@@ -4004,7 +4017,7 @@
       <c r="BN12">
         <v>15332</v>
       </c>
-      <c r="BP12" s="2">
+      <c r="BP12" s="4">
         <v>791811000.29999995</v>
       </c>
       <c r="BQ12">
@@ -4218,7 +4231,7 @@
       <c r="BN13">
         <v>41242</v>
       </c>
-      <c r="BP13" s="2">
+      <c r="BP13" s="4">
         <v>3764749</v>
       </c>
       <c r="BQ13">
@@ -4432,7 +4445,7 @@
       <c r="BN14">
         <v>219839</v>
       </c>
-      <c r="BP14" s="2">
+      <c r="BP14" s="4">
         <v>22813134.66</v>
       </c>
       <c r="BQ14">
@@ -4646,7 +4659,7 @@
       <c r="BN15">
         <v>12394</v>
       </c>
-      <c r="BP15" s="2">
+      <c r="BP15" s="4">
         <v>304306.8</v>
       </c>
       <c r="BQ15">
@@ -4863,7 +4876,7 @@
       <c r="BN16">
         <v>141251</v>
       </c>
-      <c r="BP16" s="2">
+      <c r="BP16" s="4">
         <v>4057479.94</v>
       </c>
       <c r="BQ16">
@@ -5077,7 +5090,7 @@
       <c r="BN17">
         <v>32321</v>
       </c>
-      <c r="BP17" s="2">
+      <c r="BP17" s="4">
         <v>10109437.279999999</v>
       </c>
       <c r="BQ17">
@@ -5291,7 +5304,7 @@
       <c r="BN18">
         <v>1351</v>
       </c>
-      <c r="BP18" s="2">
+      <c r="BP18" s="4">
         <v>8924661.7300000004</v>
       </c>
       <c r="BQ18">
@@ -5502,7 +5515,7 @@
       <c r="BN19">
         <v>1233</v>
       </c>
-      <c r="BP19" s="2">
+      <c r="BP19" s="4">
         <v>932727.68</v>
       </c>
       <c r="BQ19">
@@ -5728,7 +5741,7 @@
       <c r="BN20">
         <v>18000</v>
       </c>
-      <c r="BP20" s="4">
+      <c r="BP20" s="3">
         <v>842383.03949999996</v>
       </c>
       <c r="BQ20">
@@ -5954,7 +5967,7 @@
       <c r="BN21">
         <v>8000</v>
       </c>
-      <c r="BP21" s="4">
+      <c r="BP21" s="3">
         <v>6693482.6610000003</v>
       </c>
       <c r="BQ21">
@@ -6183,7 +6196,7 @@
       <c r="BN22">
         <v>1000</v>
       </c>
-      <c r="BP22" s="4">
+      <c r="BP22" s="3">
         <v>2316444.551</v>
       </c>
       <c r="BQ22">
@@ -6403,7 +6416,7 @@
       <c r="BN23">
         <v>20000</v>
       </c>
-      <c r="BP23" s="4">
+      <c r="BP23" s="3">
         <v>1584495.36</v>
       </c>
       <c r="BQ23">
@@ -6629,7 +6642,7 @@
       <c r="BN24">
         <v>20000</v>
       </c>
-      <c r="BP24" s="4">
+      <c r="BP24" s="3">
         <v>127622.9662</v>
       </c>
       <c r="BQ24">
@@ -6858,7 +6871,7 @@
       <c r="BO25">
         <v>1807645.81</v>
       </c>
-      <c r="BP25">
+      <c r="BP25" s="4">
         <v>2093791.94</v>
       </c>
       <c r="BQ25">
@@ -7087,7 +7100,7 @@
       <c r="BO26">
         <v>19151760.59</v>
       </c>
-      <c r="BP26">
+      <c r="BP26" s="4">
         <v>17000000</v>
       </c>
       <c r="BQ26">
@@ -7316,7 +7329,7 @@
       <c r="BO27">
         <v>31485709.75</v>
       </c>
-      <c r="BP27">
+      <c r="BP27" s="4">
         <v>29468459.190000001</v>
       </c>
       <c r="BQ27">
@@ -7545,7 +7558,7 @@
       <c r="BO28">
         <v>1</v>
       </c>
-      <c r="BP28">
+      <c r="BP28" s="4">
         <v>20885570.18</v>
       </c>
       <c r="BQ28">
@@ -7774,7 +7787,7 @@
       <c r="BO29">
         <v>1</v>
       </c>
-      <c r="BP29">
+      <c r="BP29" s="4">
         <v>2001800</v>
       </c>
       <c r="BQ29">
@@ -8003,7 +8016,7 @@
       <c r="BO30">
         <v>0</v>
       </c>
-      <c r="BP30">
+      <c r="BP30" s="4">
         <v>770909</v>
       </c>
       <c r="BQ30">
@@ -8226,7 +8239,7 @@
       <c r="BO31">
         <v>0</v>
       </c>
-      <c r="BP31">
+      <c r="BP31" s="4">
         <v>4082837</v>
       </c>
       <c r="BQ31">
@@ -8455,7 +8468,7 @@
       <c r="BO32">
         <v>0</v>
       </c>
-      <c r="BP32">
+      <c r="BP32" s="4">
         <v>1777799</v>
       </c>
       <c r="BQ32">
@@ -8684,7 +8697,7 @@
       <c r="BO33">
         <v>128352840</v>
       </c>
-      <c r="BP33">
+      <c r="BP33" s="4">
         <v>176393615</v>
       </c>
       <c r="BQ33">
@@ -8910,7 +8923,7 @@
       <c r="BO34">
         <v>1810670</v>
       </c>
-      <c r="BP34">
+      <c r="BP34" s="4">
         <v>0</v>
       </c>
       <c r="BQ34">
@@ -9136,7 +9149,7 @@
       <c r="BO35">
         <v>14584290</v>
       </c>
-      <c r="BP35"/>
+      <c r="BP35" s="4"/>
       <c r="BQ35">
         <v>0</v>
       </c>
@@ -9360,7 +9373,7 @@
       <c r="BN36">
         <v>12341</v>
       </c>
-      <c r="BP36">
+      <c r="BP36" s="4">
         <v>11419335.6</v>
       </c>
       <c r="BQ36">
@@ -9586,7 +9599,7 @@
       <c r="BN37">
         <v>10000</v>
       </c>
-      <c r="BP37">
+      <c r="BP37" s="4">
         <v>14013969</v>
       </c>
       <c r="BQ37">
@@ -9812,7 +9825,7 @@
       <c r="BN38">
         <v>10000</v>
       </c>
-      <c r="BP38">
+      <c r="BP38" s="4">
         <v>4680507</v>
       </c>
       <c r="BQ38">
@@ -10041,7 +10054,7 @@
       <c r="BO39">
         <v>0</v>
       </c>
-      <c r="BP39">
+      <c r="BP39" s="4">
         <v>8329834</v>
       </c>
       <c r="BQ39">
@@ -10264,7 +10277,7 @@
       <c r="BO40">
         <v>0</v>
       </c>
-      <c r="BP40">
+      <c r="BP40" s="4">
         <v>5078329</v>
       </c>
       <c r="BQ40">
@@ -10493,7 +10506,7 @@
       <c r="BO41">
         <v>0</v>
       </c>
-      <c r="BP41">
+      <c r="BP41" s="4">
         <v>28000000</v>
       </c>
       <c r="BQ41">
@@ -10719,7 +10732,7 @@
       <c r="BN42">
         <v>8000</v>
       </c>
-      <c r="BP42">
+      <c r="BP42" s="4">
         <v>8799782</v>
       </c>
       <c r="BQ42">
@@ -10948,7 +10961,7 @@
       <c r="BN43">
         <v>1000</v>
       </c>
-      <c r="BP43">
+      <c r="BP43" s="4">
         <v>1316465</v>
       </c>
       <c r="BQ43">
@@ -11168,7 +11181,7 @@
       <c r="BN44">
         <v>20000</v>
       </c>
-      <c r="BP44">
+      <c r="BP44" s="4">
         <v>1584420</v>
       </c>
       <c r="BQ44">
@@ -11394,7 +11407,7 @@
       <c r="BN45">
         <v>20000</v>
       </c>
-      <c r="BP45">
+      <c r="BP45" s="4">
         <v>19029</v>
       </c>
       <c r="BQ45">
@@ -11420,13 +11433,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE154695-4514-4425-BC50-C5F252A6A7DD}">
   <dimension ref="A1:BT45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="68" max="68" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="66" width="0" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.25">
@@ -11631,7 +11646,7 @@
       <c r="BO1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BP1" s="3" t="s">
         <v>67</v>
       </c>
       <c r="BQ1" t="s">
@@ -11848,7 +11863,7 @@
       <c r="BN2">
         <v>18000</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="4">
         <v>891186.97</v>
       </c>
       <c r="BQ2">
@@ -12026,15 +12041,15 @@
         <v>20</v>
       </c>
       <c r="BB3">
-        <f t="shared" ref="BB3:BB45" si="0">_xlfn.MAXIFS(BA:BA,E:E,E3)</f>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E3)</f>
         <v>20</v>
       </c>
       <c r="BC3">
-        <f t="shared" ref="BC3:BC19" si="1">IF(OR(BH3="SCENARIO1",BH3="SCENARIO2"),10,BA3)</f>
+        <f t="shared" ref="BC3:BC16" si="0">IF(OR(BH3="SCENARIO1",BH3="SCENARIO2"),10,BA3)</f>
         <v>10</v>
       </c>
       <c r="BD3">
-        <f t="shared" ref="BD3:BD45" si="2">_xlfn.MAXIFS(BC:BC,E:E,E3)</f>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E3)</f>
         <v>10</v>
       </c>
       <c r="BE3">
@@ -12044,7 +12059,7 @@
         <v>1</v>
       </c>
       <c r="BG3" t="str">
-        <f t="shared" ref="BG3:BG45" si="3">IF(AND(AB3 = "N", AC3 = "N", OR(Z3="Y",AD3="Y")), "SCENARIO","NA")</f>
+        <f t="shared" ref="BG3:BG45" si="1">IF(AND(AB3 = "N", AC3 = "N", OR(Z3="Y",AD3="Y")), "SCENARIO","NA")</f>
         <v>SCENARIO</v>
       </c>
       <c r="BH3" t="s">
@@ -12065,7 +12080,7 @@
       <c r="BN3">
         <v>8000</v>
       </c>
-      <c r="BP3">
+      <c r="BP3" s="4">
         <v>113431.08</v>
       </c>
       <c r="BQ3">
@@ -12246,15 +12261,15 @@
         <v>20</v>
       </c>
       <c r="BB4">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E4)</f>
+        <v>20</v>
+      </c>
+      <c r="BC4">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC4">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD4">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E4)</f>
         <v>10</v>
       </c>
       <c r="BE4">
@@ -12264,7 +12279,7 @@
         <v>1</v>
       </c>
       <c r="BG4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH4" t="s">
@@ -12285,7 +12300,7 @@
       <c r="BN4">
         <v>1000</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="4">
         <v>14744.43</v>
       </c>
       <c r="BQ4">
@@ -12401,8 +12416,8 @@
       <c r="AG5" t="b">
         <v>0</v>
       </c>
-      <c r="AH5" t="s">
-        <v>73</v>
+      <c r="AH5" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="AI5" t="s">
         <v>81</v>
@@ -12463,15 +12478,15 @@
         <v>20</v>
       </c>
       <c r="BB5">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E5)</f>
+        <v>20</v>
+      </c>
+      <c r="BC5">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC5">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD5">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E5)</f>
         <v>10</v>
       </c>
       <c r="BE5">
@@ -12481,7 +12496,7 @@
         <v>1</v>
       </c>
       <c r="BG5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH5" t="s">
@@ -12502,7 +12517,7 @@
       <c r="BN5">
         <v>7000</v>
       </c>
-      <c r="BP5">
+      <c r="BP5" s="4">
         <v>324680.8</v>
       </c>
       <c r="BQ5">
@@ -12680,15 +12695,15 @@
         <v>20</v>
       </c>
       <c r="BB6">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E6)</f>
+        <v>20</v>
+      </c>
+      <c r="BC6">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC6">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD6">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E6)</f>
         <v>10</v>
       </c>
       <c r="BE6">
@@ -12698,7 +12713,7 @@
         <v>1</v>
       </c>
       <c r="BG6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH6" t="s">
@@ -12719,7 +12734,7 @@
       <c r="BN6">
         <v>20000</v>
       </c>
-      <c r="BP6">
+      <c r="BP6" s="4">
         <v>4850034.55</v>
       </c>
       <c r="BQ6">
@@ -12888,15 +12903,15 @@
         <v>20</v>
       </c>
       <c r="BB7">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E7)</f>
+        <v>20</v>
+      </c>
+      <c r="BC7">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC7">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD7">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E7)</f>
         <v>10</v>
       </c>
       <c r="BE7">
@@ -12906,7 +12921,7 @@
         <v>1</v>
       </c>
       <c r="BG7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH7" t="s">
@@ -12928,9 +12943,9 @@
         <v>88</v>
       </c>
       <c r="BO7">
-        <v>980316320.20000005</v>
-      </c>
-      <c r="BP7"/>
+        <v>18031632.199999999</v>
+      </c>
+      <c r="BP7" s="4"/>
       <c r="BQ7">
         <v>0</v>
       </c>
@@ -13103,15 +13118,15 @@
         <v>20</v>
       </c>
       <c r="BB8">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E8)</f>
+        <v>20</v>
+      </c>
+      <c r="BC8">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC8">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD8">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E8)</f>
         <v>10</v>
       </c>
       <c r="BE8">
@@ -13121,7 +13136,7 @@
         <v>1</v>
       </c>
       <c r="BG8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH8" t="s">
@@ -13142,7 +13157,7 @@
       <c r="BN8">
         <v>50000</v>
       </c>
-      <c r="BP8" s="2">
+      <c r="BP8" s="4">
         <v>12396987.9</v>
       </c>
       <c r="BQ8">
@@ -13317,15 +13332,15 @@
         <v>20</v>
       </c>
       <c r="BB9">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E9)</f>
+        <v>20</v>
+      </c>
+      <c r="BC9">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC9">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD9">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E9)</f>
         <v>10</v>
       </c>
       <c r="BE9">
@@ -13335,7 +13350,7 @@
         <v>1</v>
       </c>
       <c r="BG9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH9" t="s">
@@ -13356,7 +13371,7 @@
       <c r="BN9">
         <v>119912</v>
       </c>
-      <c r="BP9" s="2">
+      <c r="BP9" s="4">
         <v>11103288</v>
       </c>
       <c r="BQ9">
@@ -13534,15 +13549,15 @@
         <v>20</v>
       </c>
       <c r="BB10">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E10)</f>
+        <v>20</v>
+      </c>
+      <c r="BC10">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC10">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD10">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E10)</f>
         <v>10</v>
       </c>
       <c r="BE10">
@@ -13552,7 +13567,7 @@
         <v>1</v>
       </c>
       <c r="BG10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH10" t="s">
@@ -13573,7 +13588,7 @@
       <c r="BN10">
         <v>129819</v>
       </c>
-      <c r="BP10" s="2">
+      <c r="BP10" s="4">
         <v>15094847.359999999</v>
       </c>
       <c r="BQ10">
@@ -13748,15 +13763,15 @@
         <v>20</v>
       </c>
       <c r="BB11">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E11)</f>
+        <v>20</v>
+      </c>
+      <c r="BC11">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC11">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD11">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E11)</f>
         <v>10</v>
       </c>
       <c r="BE11">
@@ -13766,7 +13781,7 @@
         <v>1</v>
       </c>
       <c r="BG11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH11" t="s">
@@ -13787,7 +13802,7 @@
       <c r="BN11">
         <v>21124</v>
       </c>
-      <c r="BP11" s="2">
+      <c r="BP11" s="4">
         <v>5849007.2999999998</v>
       </c>
       <c r="BQ11">
@@ -13900,7 +13915,7 @@
       <c r="AG12" t="b">
         <v>0</v>
       </c>
-      <c r="AH12" s="3" t="s">
+      <c r="AH12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AI12" t="s">
@@ -13959,15 +13974,15 @@
         <v>20</v>
       </c>
       <c r="BB12">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E12)</f>
+        <v>20</v>
+      </c>
+      <c r="BC12">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC12">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD12">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E12)</f>
         <v>10</v>
       </c>
       <c r="BE12">
@@ -13977,7 +13992,7 @@
         <v>1</v>
       </c>
       <c r="BG12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH12" t="s">
@@ -13998,7 +14013,7 @@
       <c r="BN12">
         <v>15332</v>
       </c>
-      <c r="BP12" s="2">
+      <c r="BP12" s="4">
         <v>791811000.29999995</v>
       </c>
       <c r="BQ12">
@@ -14173,15 +14188,15 @@
         <v>20</v>
       </c>
       <c r="BB13">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E13)</f>
+        <v>20</v>
+      </c>
+      <c r="BC13">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC13">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD13">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E13)</f>
         <v>10</v>
       </c>
       <c r="BE13">
@@ -14191,7 +14206,7 @@
         <v>1</v>
       </c>
       <c r="BG13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH13" t="s">
@@ -14212,7 +14227,7 @@
       <c r="BN13">
         <v>41242</v>
       </c>
-      <c r="BP13" s="2">
+      <c r="BP13" s="4">
         <v>3764749</v>
       </c>
       <c r="BQ13">
@@ -14387,15 +14402,15 @@
         <v>20</v>
       </c>
       <c r="BB14">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E14)</f>
+        <v>20</v>
+      </c>
+      <c r="BC14">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC14">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="BD14">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E14)</f>
         <v>10</v>
       </c>
       <c r="BE14">
@@ -14405,7 +14420,7 @@
         <v>1</v>
       </c>
       <c r="BG14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH14" t="s">
@@ -14426,7 +14441,7 @@
       <c r="BN14">
         <v>219839</v>
       </c>
-      <c r="BP14" s="2">
+      <c r="BP14" s="4">
         <v>22813134.66</v>
       </c>
       <c r="BQ14">
@@ -14601,25 +14616,25 @@
         <v>10</v>
       </c>
       <c r="BB15">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E15)</f>
+        <v>20</v>
+      </c>
+      <c r="BC15">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC15">
+        <v>10</v>
+      </c>
+      <c r="BD15">
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E15)</f>
+        <v>10</v>
+      </c>
+      <c r="BE15">
+        <v>20</v>
+      </c>
+      <c r="BF15">
+        <v>1</v>
+      </c>
+      <c r="BG15" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="BD15">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="BE15">
-        <v>20</v>
-      </c>
-      <c r="BF15">
-        <v>1</v>
-      </c>
-      <c r="BG15" t="str">
-        <f t="shared" si="3"/>
         <v>NA</v>
       </c>
       <c r="BH15" t="s">
@@ -14640,7 +14655,7 @@
       <c r="BN15">
         <v>12394</v>
       </c>
-      <c r="BP15" s="2">
+      <c r="BP15" s="4">
         <v>304306.8</v>
       </c>
       <c r="BQ15">
@@ -14818,25 +14833,25 @@
         <v>10</v>
       </c>
       <c r="BB16">
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E16)</f>
+        <v>20</v>
+      </c>
+      <c r="BC16">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="BC16">
+        <v>10</v>
+      </c>
+      <c r="BD16">
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E16)</f>
+        <v>10</v>
+      </c>
+      <c r="BE16">
+        <v>20</v>
+      </c>
+      <c r="BF16">
+        <v>1</v>
+      </c>
+      <c r="BG16" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="BD16">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="BE16">
-        <v>20</v>
-      </c>
-      <c r="BF16">
-        <v>1</v>
-      </c>
-      <c r="BG16" t="str">
-        <f t="shared" si="3"/>
         <v>NA</v>
       </c>
       <c r="BH16" t="s">
@@ -14857,7 +14872,7 @@
       <c r="BN16">
         <v>141251</v>
       </c>
-      <c r="BP16" s="2">
+      <c r="BP16" s="4">
         <v>4057479.94</v>
       </c>
       <c r="BQ16">
@@ -15032,7 +15047,7 @@
         <v>10</v>
       </c>
       <c r="BB17">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E17)</f>
         <v>20</v>
       </c>
       <c r="BC17">
@@ -15040,7 +15055,7 @@
         <v>10</v>
       </c>
       <c r="BD17">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E17)</f>
         <v>10</v>
       </c>
       <c r="BE17">
@@ -15050,7 +15065,7 @@
         <v>1</v>
       </c>
       <c r="BG17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="BH17" t="s">
@@ -15071,7 +15086,7 @@
       <c r="BN17">
         <v>32321</v>
       </c>
-      <c r="BP17" s="2">
+      <c r="BP17" s="4">
         <v>10109437.279999999</v>
       </c>
       <c r="BQ17">
@@ -15166,7 +15181,7 @@
       <c r="Z18" t="s">
         <v>81</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AA18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AB18" t="s">
@@ -15246,15 +15261,15 @@
         <v>20</v>
       </c>
       <c r="BB18">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E18)</f>
         <v>20</v>
       </c>
       <c r="BC18">
-        <f t="shared" ref="BC18:BC34" si="4">IF(OR(BH18="SCENARIO1",BH18="SCENARIO2"),10,BA18)</f>
+        <f t="shared" ref="BC18:BC19" si="2">IF(OR(BH18="SCENARIO1",BH18="SCENARIO2"),10,BA18)</f>
         <v>10</v>
       </c>
       <c r="BD18">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E18)</f>
         <v>10</v>
       </c>
       <c r="BE18">
@@ -15264,7 +15279,7 @@
         <v>1</v>
       </c>
       <c r="BG18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="BH18" t="s">
@@ -15285,7 +15300,7 @@
       <c r="BN18">
         <v>1351</v>
       </c>
-      <c r="BP18" s="2">
+      <c r="BP18" s="4">
         <v>8924661.7300000004</v>
       </c>
       <c r="BQ18">
@@ -15457,17 +15472,17 @@
         <v>10</v>
       </c>
       <c r="BB19">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E19)</f>
         <v>20</v>
       </c>
       <c r="BC19">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="BD19">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="BD19">
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E19)</f>
+        <v>10</v>
+      </c>
       <c r="BE19">
         <v>20</v>
       </c>
@@ -15475,7 +15490,7 @@
         <v>1</v>
       </c>
       <c r="BG19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="BH19" t="s">
@@ -15496,7 +15511,7 @@
       <c r="BN19">
         <v>1233</v>
       </c>
-      <c r="BP19" s="2">
+      <c r="BP19" s="4">
         <v>932727.68</v>
       </c>
       <c r="BQ19">
@@ -15680,7 +15695,7 @@
         <v>20</v>
       </c>
       <c r="BB20">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E20)</f>
         <v>20</v>
       </c>
       <c r="BC20">
@@ -15688,7 +15703,7 @@
         <v>5</v>
       </c>
       <c r="BD20">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E20)</f>
         <v>5</v>
       </c>
       <c r="BE20">
@@ -15698,7 +15713,7 @@
         <v>1</v>
       </c>
       <c r="BG20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH20" t="s">
@@ -15722,7 +15737,7 @@
       <c r="BN20">
         <v>18000</v>
       </c>
-      <c r="BP20" s="4">
+      <c r="BP20" s="3">
         <v>842383.03949999996</v>
       </c>
       <c r="BQ20">
@@ -15906,15 +15921,15 @@
         <v>20</v>
       </c>
       <c r="BB21">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E21)</f>
         <v>20</v>
       </c>
       <c r="BC21">
-        <f t="shared" ref="BC21:BC45" si="5">IF(OR(BH21="SCENARIO1",BH21="SCENARIO2"),5,BA21)</f>
+        <f t="shared" ref="BC21:BC45" si="3">IF(OR(BH21="SCENARIO1",BH21="SCENARIO2"),5,BA21)</f>
         <v>5</v>
       </c>
       <c r="BD21">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E21)</f>
         <v>5</v>
       </c>
       <c r="BE21">
@@ -15924,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="BG21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH21" t="s">
@@ -15948,7 +15963,7 @@
       <c r="BN21">
         <v>8000</v>
       </c>
-      <c r="BP21" s="4">
+      <c r="BP21" s="3">
         <v>8693482.6610000003</v>
       </c>
       <c r="BQ21">
@@ -16135,15 +16150,15 @@
         <v>20</v>
       </c>
       <c r="BB22">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E22)</f>
         <v>20</v>
       </c>
       <c r="BC22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD22">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E22)</f>
         <v>5</v>
       </c>
       <c r="BE22">
@@ -16153,7 +16168,7 @@
         <v>1</v>
       </c>
       <c r="BG22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH22" t="s">
@@ -16177,7 +16192,7 @@
       <c r="BN22">
         <v>1000</v>
       </c>
-      <c r="BP22" s="4">
+      <c r="BP22" s="3">
         <v>2316444.551</v>
       </c>
       <c r="BQ22">
@@ -16358,15 +16373,15 @@
         <v>20</v>
       </c>
       <c r="BB23">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E23)</f>
         <v>20</v>
       </c>
       <c r="BC23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD23">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E23)</f>
         <v>5</v>
       </c>
       <c r="BE23">
@@ -16376,7 +16391,7 @@
         <v>1</v>
       </c>
       <c r="BG23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH23" t="s">
@@ -16397,7 +16412,7 @@
       <c r="BN23">
         <v>20000</v>
       </c>
-      <c r="BP23" s="4">
+      <c r="BP23" s="3">
         <v>1584495.36</v>
       </c>
       <c r="BQ23">
@@ -16581,15 +16596,15 @@
         <v>20</v>
       </c>
       <c r="BB24">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E24)</f>
         <v>20</v>
       </c>
       <c r="BC24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD24">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E24)</f>
         <v>5</v>
       </c>
       <c r="BE24">
@@ -16599,7 +16614,7 @@
         <v>1</v>
       </c>
       <c r="BG24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH24" t="s">
@@ -16623,7 +16638,7 @@
       <c r="BN24">
         <v>20000</v>
       </c>
-      <c r="BP24" s="4">
+      <c r="BP24" s="3">
         <v>127622.9662</v>
       </c>
       <c r="BQ24">
@@ -16718,7 +16733,7 @@
       <c r="Z25" t="s">
         <v>81</v>
       </c>
-      <c r="AA25" s="3" t="s">
+      <c r="AA25" s="2" t="s">
         <v>81</v>
       </c>
       <c r="AB25" t="s">
@@ -16807,15 +16822,15 @@
         <v>20</v>
       </c>
       <c r="BB25">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E25)</f>
         <v>20</v>
       </c>
       <c r="BC25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD25">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E25)</f>
         <v>5</v>
       </c>
       <c r="BE25">
@@ -16825,7 +16840,7 @@
         <v>1</v>
       </c>
       <c r="BG25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH25" t="s">
@@ -16852,7 +16867,7 @@
       <c r="BO25">
         <v>1807645.81</v>
       </c>
-      <c r="BP25" s="4">
+      <c r="BP25" s="3">
         <v>2093791.94</v>
       </c>
       <c r="BQ25">
@@ -17036,15 +17051,15 @@
         <v>20</v>
       </c>
       <c r="BB26">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E26)</f>
         <v>20</v>
       </c>
       <c r="BC26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD26">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E26)</f>
         <v>5</v>
       </c>
       <c r="BE26">
@@ -17054,7 +17069,7 @@
         <v>1</v>
       </c>
       <c r="BG26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH26" t="s">
@@ -17081,7 +17096,7 @@
       <c r="BO26">
         <v>19151760.59</v>
       </c>
-      <c r="BP26" s="4">
+      <c r="BP26" s="3">
         <v>17000000</v>
       </c>
       <c r="BQ26">
@@ -17265,15 +17280,15 @@
         <v>20</v>
       </c>
       <c r="BB27">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E27)</f>
         <v>20</v>
       </c>
       <c r="BC27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD27">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E27)</f>
         <v>5</v>
       </c>
       <c r="BE27">
@@ -17283,7 +17298,7 @@
         <v>1</v>
       </c>
       <c r="BG27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH27" t="s">
@@ -17310,7 +17325,7 @@
       <c r="BO27">
         <v>31485709.75</v>
       </c>
-      <c r="BP27" s="4">
+      <c r="BP27" s="3">
         <v>29468459.190000001</v>
       </c>
       <c r="BQ27">
@@ -17494,15 +17509,15 @@
         <v>20</v>
       </c>
       <c r="BB28">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E28)</f>
         <v>20</v>
       </c>
       <c r="BC28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD28">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E28)</f>
         <v>5</v>
       </c>
       <c r="BE28">
@@ -17512,7 +17527,7 @@
         <v>1</v>
       </c>
       <c r="BG28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH28" t="s">
@@ -17539,7 +17554,7 @@
       <c r="BO28">
         <v>1</v>
       </c>
-      <c r="BP28" s="4">
+      <c r="BP28" s="3">
         <v>20885570.18</v>
       </c>
       <c r="BQ28">
@@ -17723,15 +17738,15 @@
         <v>20</v>
       </c>
       <c r="BB29">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E29)</f>
         <v>20</v>
       </c>
       <c r="BC29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD29">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E29)</f>
         <v>5</v>
       </c>
       <c r="BE29">
@@ -17741,7 +17756,7 @@
         <v>1</v>
       </c>
       <c r="BG29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH29" t="s">
@@ -17863,7 +17878,7 @@
       <c r="Z30" t="s">
         <v>73</v>
       </c>
-      <c r="AA30" s="3" t="s">
+      <c r="AA30" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AB30" t="s">
@@ -17952,15 +17967,15 @@
         <v>20</v>
       </c>
       <c r="BB30">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E30)</f>
         <v>20</v>
       </c>
       <c r="BC30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD30">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E30)</f>
         <v>5</v>
       </c>
       <c r="BE30">
@@ -17970,7 +17985,7 @@
         <v>1</v>
       </c>
       <c r="BG30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH30" t="s">
@@ -17997,7 +18012,7 @@
       <c r="BO30">
         <v>0</v>
       </c>
-      <c r="BP30">
+      <c r="BP30" s="4">
         <v>770909</v>
       </c>
       <c r="BQ30">
@@ -18178,15 +18193,15 @@
         <v>20</v>
       </c>
       <c r="BB31">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E31)</f>
         <v>20</v>
       </c>
       <c r="BC31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD31">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E31)</f>
         <v>5</v>
       </c>
       <c r="BE31">
@@ -18196,7 +18211,7 @@
         <v>1</v>
       </c>
       <c r="BG31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH31" t="s">
@@ -18220,7 +18235,7 @@
       <c r="BO31">
         <v>0</v>
       </c>
-      <c r="BP31">
+      <c r="BP31" s="4">
         <v>4082837</v>
       </c>
       <c r="BQ31">
@@ -18404,15 +18419,15 @@
         <v>20</v>
       </c>
       <c r="BB32">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E32)</f>
         <v>20</v>
       </c>
       <c r="BC32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD32">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E32)</f>
         <v>5</v>
       </c>
       <c r="BE32">
@@ -18422,7 +18437,7 @@
         <v>1</v>
       </c>
       <c r="BG32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH32" t="s">
@@ -18449,7 +18464,7 @@
       <c r="BO32">
         <v>0</v>
       </c>
-      <c r="BP32">
+      <c r="BP32" s="4">
         <v>1777799</v>
       </c>
       <c r="BQ32">
@@ -18633,15 +18648,15 @@
         <v>20</v>
       </c>
       <c r="BB33">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E33)</f>
         <v>20</v>
       </c>
       <c r="BC33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD33">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E33)</f>
         <v>5</v>
       </c>
       <c r="BE33">
@@ -18651,7 +18666,7 @@
         <v>1</v>
       </c>
       <c r="BG33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH33" t="s">
@@ -18678,7 +18693,7 @@
       <c r="BO33">
         <v>128352840</v>
       </c>
-      <c r="BP33">
+      <c r="BP33" s="4">
         <v>176393615</v>
       </c>
       <c r="BQ33">
@@ -18859,15 +18874,15 @@
         <v>20</v>
       </c>
       <c r="BB34">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E34)</f>
         <v>20</v>
       </c>
       <c r="BC34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD34">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E34)</f>
         <v>5</v>
       </c>
       <c r="BE34">
@@ -18877,7 +18892,7 @@
         <v>1</v>
       </c>
       <c r="BG34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH34" t="s">
@@ -18904,7 +18919,7 @@
       <c r="BO34">
         <v>1810670</v>
       </c>
-      <c r="BP34">
+      <c r="BP34" s="4">
         <v>0</v>
       </c>
       <c r="BQ34">
@@ -19085,15 +19100,15 @@
         <v>20</v>
       </c>
       <c r="BB35">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E35)</f>
         <v>20</v>
       </c>
       <c r="BC35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD35">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E35)</f>
         <v>5</v>
       </c>
       <c r="BE35">
@@ -19103,7 +19118,7 @@
         <v>1</v>
       </c>
       <c r="BG35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH35" t="s">
@@ -19130,7 +19145,7 @@
       <c r="BO35">
         <v>14584290</v>
       </c>
-      <c r="BP35"/>
+      <c r="BP35" s="4"/>
       <c r="BQ35">
         <v>0</v>
       </c>
@@ -19312,15 +19327,15 @@
         <v>20</v>
       </c>
       <c r="BB36">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E36)</f>
         <v>20</v>
       </c>
       <c r="BC36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD36">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E36)</f>
         <v>5</v>
       </c>
       <c r="BE36">
@@ -19330,7 +19345,7 @@
         <v>1</v>
       </c>
       <c r="BG36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH36" t="s">
@@ -19354,7 +19369,7 @@
       <c r="BN36">
         <v>12341</v>
       </c>
-      <c r="BP36">
+      <c r="BP36" s="4">
         <v>11419335.6</v>
       </c>
       <c r="BQ36">
@@ -19538,15 +19553,15 @@
         <v>20</v>
       </c>
       <c r="BB37">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E37)</f>
         <v>20</v>
       </c>
       <c r="BC37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD37">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E37)</f>
         <v>5</v>
       </c>
       <c r="BE37">
@@ -19556,7 +19571,7 @@
         <v>1</v>
       </c>
       <c r="BG37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH37" t="s">
@@ -19580,7 +19595,7 @@
       <c r="BN37">
         <v>10000</v>
       </c>
-      <c r="BP37">
+      <c r="BP37" s="4">
         <v>14013969</v>
       </c>
       <c r="BQ37">
@@ -19764,15 +19779,15 @@
         <v>20</v>
       </c>
       <c r="BB38">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E38)</f>
         <v>20</v>
       </c>
       <c r="BC38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD38">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E38)</f>
         <v>5</v>
       </c>
       <c r="BE38">
@@ -19782,7 +19797,7 @@
         <v>1</v>
       </c>
       <c r="BG38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH38" t="s">
@@ -19806,7 +19821,7 @@
       <c r="BN38">
         <v>10000</v>
       </c>
-      <c r="BP38">
+      <c r="BP38" s="4">
         <v>4680507</v>
       </c>
       <c r="BQ38">
@@ -19990,15 +20005,15 @@
         <v>20</v>
       </c>
       <c r="BB39">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E39)</f>
         <v>20</v>
       </c>
       <c r="BC39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD39">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E39)</f>
         <v>5</v>
       </c>
       <c r="BE39">
@@ -20008,7 +20023,7 @@
         <v>1</v>
       </c>
       <c r="BG39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH39" t="s">
@@ -20035,7 +20050,7 @@
       <c r="BO39">
         <v>0</v>
       </c>
-      <c r="BP39">
+      <c r="BP39" s="4">
         <v>8329834</v>
       </c>
       <c r="BQ39">
@@ -20216,15 +20231,15 @@
         <v>20</v>
       </c>
       <c r="BB40">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E40)</f>
         <v>20</v>
       </c>
       <c r="BC40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD40">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E40)</f>
         <v>5</v>
       </c>
       <c r="BE40">
@@ -20234,7 +20249,7 @@
         <v>1</v>
       </c>
       <c r="BG40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH40" t="s">
@@ -20258,7 +20273,7 @@
       <c r="BO40">
         <v>0</v>
       </c>
-      <c r="BP40">
+      <c r="BP40" s="4">
         <v>5078329</v>
       </c>
       <c r="BQ40">
@@ -20442,15 +20457,15 @@
         <v>20</v>
       </c>
       <c r="BB41">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E41)</f>
         <v>20</v>
       </c>
       <c r="BC41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD41">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E41)</f>
         <v>5</v>
       </c>
       <c r="BE41">
@@ -20460,7 +20475,7 @@
         <v>1</v>
       </c>
       <c r="BG41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH41" t="s">
@@ -20487,7 +20502,7 @@
       <c r="BO41">
         <v>0</v>
       </c>
-      <c r="BP41">
+      <c r="BP41" s="4">
         <v>28000000</v>
       </c>
       <c r="BQ41">
@@ -20671,15 +20686,15 @@
         <v>20</v>
       </c>
       <c r="BB42">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E42)</f>
         <v>20</v>
       </c>
       <c r="BC42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD42">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E42)</f>
         <v>5</v>
       </c>
       <c r="BE42">
@@ -20689,7 +20704,7 @@
         <v>1</v>
       </c>
       <c r="BG42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH42" t="s">
@@ -20713,7 +20728,7 @@
       <c r="BN42">
         <v>8000</v>
       </c>
-      <c r="BP42">
+      <c r="BP42" s="4">
         <v>8799782</v>
       </c>
       <c r="BQ42">
@@ -20805,7 +20820,7 @@
       <c r="Y43" t="s">
         <v>81</v>
       </c>
-      <c r="Z43" s="3" t="s">
+      <c r="Z43" s="2" t="s">
         <v>81</v>
       </c>
       <c r="AA43" t="s">
@@ -20900,15 +20915,15 @@
         <v>20</v>
       </c>
       <c r="BB43">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E43)</f>
         <v>20</v>
       </c>
       <c r="BC43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD43">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E43)</f>
         <v>5</v>
       </c>
       <c r="BE43">
@@ -20918,7 +20933,7 @@
         <v>1</v>
       </c>
       <c r="BG43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH43" t="s">
@@ -20942,7 +20957,7 @@
       <c r="BN43">
         <v>1000</v>
       </c>
-      <c r="BP43">
+      <c r="BP43" s="4">
         <v>1316465</v>
       </c>
       <c r="BQ43">
@@ -21123,15 +21138,15 @@
         <v>20</v>
       </c>
       <c r="BB44">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E44)</f>
         <v>20</v>
       </c>
       <c r="BC44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD44">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E44)</f>
         <v>5</v>
       </c>
       <c r="BE44">
@@ -21141,7 +21156,7 @@
         <v>1</v>
       </c>
       <c r="BG44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH44" t="s">
@@ -21162,7 +21177,7 @@
       <c r="BN44">
         <v>20000</v>
       </c>
-      <c r="BP44">
+      <c r="BP44" s="4">
         <v>1584420</v>
       </c>
       <c r="BQ44">
@@ -21346,15 +21361,15 @@
         <v>20</v>
       </c>
       <c r="BB45">
-        <f t="shared" si="0"/>
+        <f>_xlfn.MAXIFS(BA:BA,E:E,E45)</f>
         <v>20</v>
       </c>
       <c r="BC45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="BD45">
-        <f t="shared" si="2"/>
+        <f>_xlfn.MAXIFS(BC:BC,E:E,E45)</f>
         <v>5</v>
       </c>
       <c r="BE45">
@@ -21364,7 +21379,7 @@
         <v>1</v>
       </c>
       <c r="BG45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>SCENARIO</v>
       </c>
       <c r="BH45" t="s">
@@ -21388,7 +21403,7 @@
       <c r="BN45">
         <v>20000</v>
       </c>
-      <c r="BP45">
+      <c r="BP45" s="4">
         <v>19029</v>
       </c>
       <c r="BQ45">

</xml_diff>